<commit_message>
(i) Edited TestScriptTax.m so that it is up to date with TestScriptOil.m and made sure it ran without problems (ii) Edited data files in Tax folder so that they run without issues
</commit_message>
<xml_diff>
--- a/Data/Tax/Data.xlsx
+++ b/Data/Tax/Data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hamzahusain/Library/Mobile Documents/com~apple~CloudDocs/Desktop/RA/SVARIV/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hamzahusain/Library/Mobile Documents/com~apple~CloudDocs/Desktop/RA/SVARIV/Data/Tax/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,42 +27,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>LogIncome</t>
-  </si>
-  <si>
-    <t>LOG RGDP</t>
-  </si>
-  <si>
-    <t>UNRATE</t>
-  </si>
-  <si>
-    <t>INFLATION</t>
-  </si>
-  <si>
-    <t>FFR</t>
-  </si>
-  <si>
-    <t>LOG GOV</t>
-  </si>
-  <si>
-    <t>LOG RSTPRICES</t>
-  </si>
-  <si>
-    <t>DLOG RDEBT</t>
-  </si>
-  <si>
-    <t>Log(1/1-AMTR)</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -96,7 +68,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,10 +346,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -389,1742 +361,1713 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
+      <c r="A1" s="2">
+        <v>0.21249979731294261</v>
+      </c>
+      <c r="B1" s="1">
+        <v>10.098128001766774</v>
+      </c>
+      <c r="C1" s="1">
+        <v>-8.3242549697164741</v>
+      </c>
+      <c r="D1" s="1">
+        <v>5.2000000000000005E-2</v>
+      </c>
+      <c r="E1" s="1">
+        <v>9.7497242265332743E-3</v>
+      </c>
+      <c r="F1" s="1">
+        <v>1.0411904597846007E-2</v>
+      </c>
+      <c r="G1" s="1">
+        <v>-12.020993958695611</v>
+      </c>
+      <c r="H1" s="1">
+        <v>5.0300723603246436</v>
+      </c>
+      <c r="I1" s="1">
+        <v>-2.9849961863623875E-2</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>0.21249979731294261</v>
+        <v>0.27303883413088065</v>
       </c>
       <c r="B2" s="1">
-        <v>10.098128001766774</v>
+        <v>10.127959435866686</v>
       </c>
       <c r="C2" s="1">
-        <v>-8.3242549697164741</v>
+        <v>-8.2565119828994504</v>
       </c>
       <c r="D2" s="1">
-        <v>5.2000000000000005E-2</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="E2" s="1">
-        <v>9.7497242265332743E-3</v>
+        <v>7.6089339285791951E-2</v>
       </c>
       <c r="F2" s="1">
-        <v>1.0411904597846007E-2</v>
+        <v>1.2132195400797314E-2</v>
       </c>
       <c r="G2" s="1">
-        <v>-12.020993958695611</v>
+        <v>-11.773242345119778</v>
       </c>
       <c r="H2" s="1">
-        <v>5.0300723603246436</v>
+        <v>5.1477873112279937</v>
       </c>
       <c r="I2" s="1">
-        <v>-2.9849961863623875E-2</v>
+        <v>-8.7897297316671175E-2</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>0.27303883413088065</v>
+        <v>0.30386197538383281</v>
       </c>
       <c r="B3" s="1">
-        <v>10.127959435866686</v>
+        <v>10.159393750175562</v>
       </c>
       <c r="C3" s="1">
-        <v>-8.2565119828994504</v>
+        <v>-8.2264793296968861</v>
       </c>
       <c r="D3" s="1">
-        <v>3.3000000000000002E-2</v>
+        <v>0.03</v>
       </c>
       <c r="E3" s="1">
-        <v>7.6089339285791951E-2</v>
+        <v>2.1619011076526196E-2</v>
       </c>
       <c r="F3" s="1">
-        <v>1.2132195400797314E-2</v>
+        <v>1.466466995502985E-2</v>
       </c>
       <c r="G3" s="1">
-        <v>-11.773242345119778</v>
+        <v>-11.614759671760115</v>
       </c>
       <c r="H3" s="1">
-        <v>5.1477873112279937</v>
+        <v>5.2185844168752222</v>
       </c>
       <c r="I3" s="1">
-        <v>-8.7897297316671175E-2</v>
+        <v>-6.940925556918387E-3</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>0.30386197538383281</v>
+        <v>0.30481721570699488</v>
       </c>
       <c r="B4" s="1">
-        <v>10.159393750175562</v>
+        <v>10.202999126975673</v>
       </c>
       <c r="C4" s="1">
-        <v>-8.2264793296968861</v>
+        <v>-8.1897905121613235</v>
       </c>
       <c r="D4" s="1">
-        <v>0.03</v>
+        <v>2.8999999999999998E-2</v>
       </c>
       <c r="E4" s="1">
-        <v>2.1619011076526196E-2</v>
+        <v>7.5157866732087266E-3</v>
       </c>
       <c r="F4" s="1">
-        <v>1.466466995502985E-2</v>
+        <v>1.6520125422106947E-2</v>
       </c>
       <c r="G4" s="1">
-        <v>-11.614759671760115</v>
+        <v>-11.563100978316013</v>
       </c>
       <c r="H4" s="1">
-        <v>5.2185844168752222</v>
+        <v>5.2205820324641579</v>
       </c>
       <c r="I4" s="1">
-        <v>-6.940925556918387E-3</v>
+        <v>1.4490150809935542E-2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>0.30481721570699488</v>
+        <v>0.26463951495565374</v>
       </c>
       <c r="B5" s="1">
-        <v>10.202999126975673</v>
+        <v>10.190783422929217</v>
       </c>
       <c r="C5" s="1">
-        <v>-8.1897905121613235</v>
+        <v>-8.2056104669049912</v>
       </c>
       <c r="D5" s="1">
-        <v>2.8999999999999998E-2</v>
+        <v>5.5999999999999994E-2</v>
       </c>
       <c r="E5" s="1">
-        <v>7.5157866732087266E-3</v>
+        <v>4.9792217658409816E-3</v>
       </c>
       <c r="F5" s="1">
-        <v>1.6520125422106947E-2</v>
+        <v>9.9576381867676218E-3</v>
       </c>
       <c r="G5" s="1">
-        <v>-11.563100978316013</v>
+        <v>-11.650541379202805</v>
       </c>
       <c r="H5" s="1">
-        <v>5.2205820324641579</v>
+        <v>5.3983005574782625</v>
       </c>
       <c r="I5" s="1">
-        <v>1.4490150809935542E-2</v>
+        <v>-4.6770763581300834E-3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>0.26463951495565374</v>
+        <v>0.27371237390330394</v>
       </c>
       <c r="B6" s="1">
-        <v>10.190783422929217</v>
+        <v>10.257247083510356</v>
       </c>
       <c r="C6" s="1">
-        <v>-8.2056104669049912</v>
+        <v>-8.1469417082541629</v>
       </c>
       <c r="D6" s="1">
-        <v>5.5999999999999994E-2</v>
+        <v>4.4000000000000004E-2</v>
       </c>
       <c r="E6" s="1">
-        <v>4.9792217658409816E-3</v>
+        <v>-3.7273437856207266E-3</v>
       </c>
       <c r="F6" s="1">
-        <v>9.9576381867676218E-3</v>
+        <v>1.7684999369606914E-2</v>
       </c>
       <c r="G6" s="1">
-        <v>-11.650541379202805</v>
+        <v>-11.675539230019503</v>
       </c>
       <c r="H6" s="1">
-        <v>5.3983005574782625</v>
+        <v>5.7123830322033955</v>
       </c>
       <c r="I6" s="1">
-        <v>-4.6770763581300834E-3</v>
+        <v>-9.9071314818846012E-3</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>0.27371237390330394</v>
+        <v>0.27528799060557307</v>
       </c>
       <c r="B7" s="1">
-        <v>10.257247083510356</v>
+        <v>10.307891221983198</v>
       </c>
       <c r="C7" s="1">
-        <v>-8.1469417082541629</v>
+        <v>-8.1359749914960915</v>
       </c>
       <c r="D7" s="1">
-        <v>4.4000000000000004E-2</v>
+        <v>4.0999999999999995E-2</v>
       </c>
       <c r="E7" s="1">
-        <v>-3.7273437856207266E-3</v>
+        <v>1.4840887213980195E-2</v>
       </c>
       <c r="F7" s="1">
-        <v>1.7684999369606914E-2</v>
+        <v>2.6916506429460588E-2</v>
       </c>
       <c r="G7" s="1">
-        <v>-11.675539230019503</v>
+        <v>-11.661082660941643</v>
       </c>
       <c r="H7" s="1">
-        <v>5.7123830322033955</v>
+        <v>5.8385059246030799</v>
       </c>
       <c r="I7" s="1">
-        <v>-9.9071314818846012E-3</v>
+        <v>-5.0958421609691218E-2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>0.27528799060557307</v>
+        <v>0.27800818516062059</v>
       </c>
       <c r="B8" s="1">
-        <v>10.307891221983198</v>
+        <v>10.312441217367136</v>
       </c>
       <c r="C8" s="1">
-        <v>-8.1359749914960915</v>
+        <v>-8.1255268078267058</v>
       </c>
       <c r="D8" s="1">
-        <v>4.0999999999999995E-2</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="E8" s="1">
-        <v>1.4840887213980195E-2</v>
+        <v>3.5009590862558518E-2</v>
       </c>
       <c r="F8" s="1">
-        <v>2.6916506429460588E-2</v>
+        <v>3.0576771872730564E-2</v>
       </c>
       <c r="G8" s="1">
-        <v>-11.661082660941643</v>
+        <v>-11.600193665982587</v>
       </c>
       <c r="H8" s="1">
-        <v>5.8385059246030799</v>
+        <v>5.7541841201218658</v>
       </c>
       <c r="I8" s="1">
-        <v>-5.0958421609691218E-2</v>
+        <v>-5.5390702798352009E-2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>0.27800818516062059</v>
+        <v>0.27565760659639871</v>
       </c>
       <c r="B9" s="1">
-        <v>10.312441217367136</v>
+        <v>10.28133524704884</v>
       </c>
       <c r="C9" s="1">
-        <v>-8.1255268078267058</v>
+        <v>-8.141774786430755</v>
       </c>
       <c r="D9" s="1">
-        <v>4.2999999999999997E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="E9" s="1">
-        <v>3.5009590862558518E-2</v>
+        <v>2.6916669794969355E-2</v>
       </c>
       <c r="F9" s="1">
-        <v>3.0576771872730564E-2</v>
+        <v>1.5591786485497562E-2</v>
       </c>
       <c r="G9" s="1">
-        <v>-11.600193665982587</v>
+        <v>-11.548420903831804</v>
       </c>
       <c r="H9" s="1">
-        <v>5.7541841201218658</v>
+        <v>5.7682877127076795</v>
       </c>
       <c r="I9" s="1">
-        <v>-5.5390702798352009E-2</v>
+        <v>4.8069424483387913E-3</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>0.27565760659639871</v>
+        <v>0.28320139114564569</v>
       </c>
       <c r="B10" s="1">
-        <v>10.28133524704884</v>
+        <v>10.33973850203847</v>
       </c>
       <c r="C10" s="1">
-        <v>-8.141774786430755</v>
+        <v>-8.0838542155179134</v>
       </c>
       <c r="D10" s="1">
-        <v>6.8000000000000005E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="E10" s="1">
-        <v>2.6916669794969355E-2</v>
+        <v>6.8949877514191691E-3</v>
       </c>
       <c r="F10" s="1">
-        <v>1.5591786485497562E-2</v>
+        <v>3.25023227191827E-2</v>
       </c>
       <c r="G10" s="1">
-        <v>-11.548420903831804</v>
+        <v>-11.50537820183102</v>
       </c>
       <c r="H10" s="1">
-        <v>5.7682877127076795</v>
+        <v>5.9772648324561644</v>
       </c>
       <c r="I10" s="1">
-        <v>4.8069424483387913E-3</v>
+        <v>1.3806542074575656E-2</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>0.28320139114564569</v>
+        <v>0.28130443579128483</v>
       </c>
       <c r="B11" s="1">
-        <v>10.33973850203847</v>
+        <v>10.350960883826643</v>
       </c>
       <c r="C11" s="1">
-        <v>-8.0838542155179134</v>
+        <v>-8.0663881291441726</v>
       </c>
       <c r="D11" s="1">
         <v>5.5E-2</v>
       </c>
       <c r="E11" s="1">
-        <v>6.8949877514191691E-3</v>
+        <v>1.7046530697499833E-2</v>
       </c>
       <c r="F11" s="1">
-        <v>3.25023227191827E-2</v>
+        <v>3.1632473904486751E-2</v>
       </c>
       <c r="G11" s="1">
-        <v>-11.50537820183102</v>
+        <v>-11.526280444825687</v>
       </c>
       <c r="H11" s="1">
-        <v>5.9772648324561644</v>
+        <v>5.9332065398887401</v>
       </c>
       <c r="I11" s="1">
-        <v>1.3806542074575656E-2</v>
+        <v>-3.3480619680279489E-2</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>0.28130443579128483</v>
+        <v>0.28368350579674806</v>
       </c>
       <c r="B12" s="1">
-        <v>10.350960883826643</v>
+        <v>10.362591170039336</v>
       </c>
       <c r="C12" s="1">
-        <v>-8.0663881291441726</v>
+        <v>-8.0601364057302582</v>
       </c>
       <c r="D12" s="1">
-        <v>5.5E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="E12" s="1">
-        <v>1.7046530697499833E-2</v>
+        <v>1.0080842819097742E-2</v>
       </c>
       <c r="F12" s="1">
-        <v>3.1632473904486751E-2</v>
+        <v>1.935747020345956E-2</v>
       </c>
       <c r="G12" s="1">
-        <v>-11.526280444825687</v>
+        <v>-11.473999400986139</v>
       </c>
       <c r="H12" s="1">
-        <v>5.9332065398887401</v>
+        <v>6.0942312014035585</v>
       </c>
       <c r="I12" s="1">
-        <v>-3.3480619680279489E-2</v>
+        <v>9.4066067518649987E-4</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>0.28368350579674806</v>
+        <v>0.28939443665405912</v>
       </c>
       <c r="B13" s="1">
-        <v>10.362591170039336</v>
+        <v>10.398462292493031</v>
       </c>
       <c r="C13" s="1">
-        <v>-8.0601364057302582</v>
+        <v>-8.0185883718362376</v>
       </c>
       <c r="D13" s="1">
-        <v>6.7000000000000004E-2</v>
+        <v>5.5999999999999994E-2</v>
       </c>
       <c r="E13" s="1">
-        <v>1.0080842819097742E-2</v>
+        <v>9.9855969456356958E-3</v>
       </c>
       <c r="F13" s="1">
-        <v>1.935747020345956E-2</v>
+        <v>2.6721422327976273E-2</v>
       </c>
       <c r="G13" s="1">
-        <v>-11.473999400986139</v>
+        <v>-11.419766065293846</v>
       </c>
       <c r="H13" s="1">
-        <v>6.0942312014035585</v>
+        <v>6.0237553619331337</v>
       </c>
       <c r="I13" s="1">
-        <v>9.4066067518649987E-4</v>
+        <v>9.3061355042944882E-5</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>0.28939443665405912</v>
+        <v>0.29956736524038952</v>
       </c>
       <c r="B14" s="1">
-        <v>10.398462292493031</v>
+        <v>10.423231447855194</v>
       </c>
       <c r="C14" s="1">
-        <v>-8.0185883718362376</v>
+        <v>-7.9927909809686506</v>
       </c>
       <c r="D14" s="1">
         <v>5.5999999999999994E-2</v>
       </c>
       <c r="E14" s="1">
-        <v>9.9855969456356958E-3</v>
+        <v>1.316079918768805E-2</v>
       </c>
       <c r="F14" s="1">
-        <v>2.6721422327976273E-2</v>
+        <v>3.1286470171036557E-2</v>
       </c>
       <c r="G14" s="1">
-        <v>-11.419766065293846</v>
+        <v>-11.417276124950703</v>
       </c>
       <c r="H14" s="1">
-        <v>6.0237553619331337</v>
+        <v>6.12387458395352</v>
       </c>
       <c r="I14" s="1">
-        <v>9.3061355042944882E-5</v>
+        <v>-1.4904620157125681E-2</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>0.29956736524038952</v>
+        <v>0.26756701738606686</v>
       </c>
       <c r="B15" s="1">
-        <v>10.423231447855194</v>
+        <v>10.470311755261182</v>
       </c>
       <c r="C15" s="1">
-        <v>-7.9927909809686506</v>
+        <v>-7.9530829292972287</v>
       </c>
       <c r="D15" s="1">
-        <v>5.5999999999999994E-2</v>
+        <v>5.2000000000000005E-2</v>
       </c>
       <c r="E15" s="1">
-        <v>1.316079918768805E-2</v>
+        <v>1.2973528943516567E-2</v>
       </c>
       <c r="F15" s="1">
-        <v>3.1286470171036557E-2</v>
+        <v>3.4369113268392176E-2</v>
       </c>
       <c r="G15" s="1">
-        <v>-11.417276124950703</v>
+        <v>-11.411177611969853</v>
       </c>
       <c r="H15" s="1">
-        <v>6.12387458395352</v>
+        <v>6.2633224184070535</v>
       </c>
       <c r="I15" s="1">
-        <v>-1.4904620157125681E-2</v>
+        <v>-5.770645045067635E-3</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>0.26756701738606686</v>
+        <v>0.25701694892598775</v>
       </c>
       <c r="B16" s="1">
-        <v>10.470311755261182</v>
+        <v>10.510465461419367</v>
       </c>
       <c r="C16" s="1">
-        <v>-7.9530829292972287</v>
+        <v>-7.9051114133184308</v>
       </c>
       <c r="D16" s="1">
-        <v>5.2000000000000005E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="E16" s="1">
-        <v>1.2973528943516567E-2</v>
+        <v>1.6000107331230407E-2</v>
       </c>
       <c r="F16" s="1">
-        <v>3.4369113268392176E-2</v>
+        <v>3.9917369616960061E-2</v>
       </c>
       <c r="G16" s="1">
-        <v>-11.411177611969853</v>
+        <v>-11.397305498101776</v>
       </c>
       <c r="H16" s="1">
-        <v>6.2633224184070535</v>
+        <v>6.3276029082452965</v>
       </c>
       <c r="I16" s="1">
-        <v>-5.770645045067635E-3</v>
+        <v>-2.4747921141501816E-2</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>0.25701694892598775</v>
+        <v>0.27834389218427102</v>
       </c>
       <c r="B17" s="1">
-        <v>10.510465461419367</v>
+        <v>10.553769832958004</v>
       </c>
       <c r="C17" s="1">
-        <v>-7.9051114133184308</v>
+        <v>-7.8553040238134928</v>
       </c>
       <c r="D17" s="1">
-        <v>4.4999999999999998E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="E17" s="1">
-        <v>1.6000107331230407E-2</v>
+        <v>2.8183935099185486E-2</v>
       </c>
       <c r="F17" s="1">
-        <v>3.9917369616960061E-2</v>
+        <v>4.9837913689734621E-2</v>
       </c>
       <c r="G17" s="1">
-        <v>-11.397305498101776</v>
+        <v>-11.292123501602681</v>
       </c>
       <c r="H17" s="1">
-        <v>6.3276029082452965</v>
+        <v>6.2658185185217583</v>
       </c>
       <c r="I17" s="1">
-        <v>-2.4747921141501816E-2</v>
+        <v>-2.8590044660523173E-2</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>0.27834389218427102</v>
+        <v>0.281968553629732</v>
       </c>
       <c r="B18" s="1">
-        <v>10.553769832958004</v>
+        <v>10.577783632735478</v>
       </c>
       <c r="C18" s="1">
-        <v>-7.8553040238134928</v>
+        <v>-7.841678387684472</v>
       </c>
       <c r="D18" s="1">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="E18" s="1">
-        <v>2.8183935099185486E-2</v>
+        <v>3.0391673548879922E-2</v>
       </c>
       <c r="F18" s="1">
-        <v>4.9837913689734621E-2</v>
+        <v>4.1327825095405883E-2</v>
       </c>
       <c r="G18" s="1">
-        <v>-11.292123501602681</v>
+        <v>-11.20920018839878</v>
       </c>
       <c r="H18" s="1">
-        <v>6.2658185185217583</v>
+        <v>6.3107698184732195</v>
       </c>
       <c r="I18" s="1">
-        <v>-2.8590044660523173E-2</v>
+        <v>3.8623886340243274E-3</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>0.281968553629732</v>
+        <v>0.32522859252747355</v>
       </c>
       <c r="B19" s="1">
-        <v>10.577783632735478</v>
+        <v>10.610024054461084</v>
       </c>
       <c r="C19" s="1">
-        <v>-7.841678387684472</v>
+        <v>-7.8062887433936998</v>
       </c>
       <c r="D19" s="1">
-        <v>3.7999999999999999E-2</v>
+        <v>3.6000000000000004E-2</v>
       </c>
       <c r="E19" s="1">
-        <v>3.0391673548879922E-2</v>
+        <v>4.105324943748849E-2</v>
       </c>
       <c r="F19" s="1">
-        <v>4.1327825095405883E-2</v>
+        <v>5.5013292953962671E-2</v>
       </c>
       <c r="G19" s="1">
-        <v>-11.20920018839878</v>
+        <v>-11.172673027332541</v>
       </c>
       <c r="H19" s="1">
-        <v>6.3107698184732195</v>
+        <v>6.3407331240988256</v>
       </c>
       <c r="I19" s="1">
-        <v>3.8623886340243274E-3</v>
+        <v>-9.5502921809456076E-3</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>0.32522859252747355</v>
+        <v>0.34213881121979878</v>
       </c>
       <c r="B20" s="1">
-        <v>10.610024054461084</v>
+        <v>10.624534504016712</v>
       </c>
       <c r="C20" s="1">
-        <v>-7.8062887433936998</v>
+        <v>-7.787722858632824</v>
       </c>
       <c r="D20" s="1">
-        <v>3.6000000000000004E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="E20" s="1">
-        <v>4.105324943748849E-2</v>
+        <v>5.3166388753340531E-2</v>
       </c>
       <c r="F20" s="1">
-        <v>5.5013292953962671E-2</v>
+        <v>7.8808403511637051E-2</v>
       </c>
       <c r="G20" s="1">
-        <v>-11.172673027332541</v>
+        <v>-11.179515202432098</v>
       </c>
       <c r="H20" s="1">
-        <v>6.3407331240988256</v>
+        <v>6.2788743836863841</v>
       </c>
       <c r="I20" s="1">
-        <v>-9.5502921809456076E-3</v>
+        <v>-7.6434062206736098E-2</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>0.34213881121979878</v>
+        <v>0.31896881090951529</v>
       </c>
       <c r="B21" s="1">
-        <v>10.624534504016712</v>
+        <v>10.630004145332425</v>
       </c>
       <c r="C21" s="1">
-        <v>-7.787722858632824</v>
+        <v>-7.7999590348560899</v>
       </c>
       <c r="D21" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>0.05</v>
       </c>
       <c r="E21" s="1">
-        <v>5.3166388753340531E-2</v>
+        <v>5.5643959602005161E-2</v>
       </c>
       <c r="F21" s="1">
-        <v>7.8808403511637051E-2</v>
+        <v>6.9289911295908432E-2</v>
       </c>
       <c r="G21" s="1">
-        <v>-11.179515202432098</v>
+        <v>-11.152212246020271</v>
       </c>
       <c r="H21" s="1">
-        <v>6.2788743836863841</v>
+        <v>6.0613846362602573</v>
       </c>
       <c r="I21" s="1">
-        <v>-7.6434062206736098E-2</v>
+        <v>-2.8786646154084217E-2</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>0.31896881090951529</v>
+        <v>0.3040277110626815</v>
       </c>
       <c r="B22" s="1">
-        <v>10.630004145332425</v>
+        <v>10.627261716452267</v>
       </c>
       <c r="C22" s="1">
-        <v>-7.7999590348560899</v>
+        <v>-7.7911981665181971</v>
       </c>
       <c r="D22" s="1">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="E22" s="1">
-        <v>5.5643959602005161E-2</v>
+        <v>4.287311570557404E-2</v>
       </c>
       <c r="F22" s="1">
-        <v>6.9289911295908432E-2</v>
+        <v>4.5539665762005195E-2</v>
       </c>
       <c r="G22" s="1">
-        <v>-11.152212246020271</v>
+        <v>-11.144812869197926</v>
       </c>
       <c r="H22" s="1">
-        <v>6.0613846362602573</v>
+        <v>6.1848782807782916</v>
       </c>
       <c r="I22" s="1">
-        <v>-2.8786646154084217E-2</v>
+        <v>1.3109614759799548E-2</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>0.3040277110626815</v>
+        <v>0.31609548991384695</v>
       </c>
       <c r="B23" s="1">
-        <v>10.627261716452267</v>
+        <v>10.667912115941821</v>
       </c>
       <c r="C23" s="1">
-        <v>-7.7911981665181971</v>
+        <v>-7.7620317288752894</v>
       </c>
       <c r="D23" s="1">
-        <v>0.06</v>
+        <v>5.5999999999999994E-2</v>
       </c>
       <c r="E23" s="1">
-        <v>4.287311570557404E-2</v>
+        <v>3.1599513754660913E-2</v>
       </c>
       <c r="F23" s="1">
-        <v>4.5539665762005195E-2</v>
+        <v>4.3338554257067265E-2</v>
       </c>
       <c r="G23" s="1">
-        <v>-11.144812869197926</v>
+        <v>-11.098364010275084</v>
       </c>
       <c r="H23" s="1">
-        <v>6.1848782807782916</v>
+        <v>6.2586816762206876</v>
       </c>
       <c r="I23" s="1">
-        <v>1.3109614759799548E-2</v>
+        <v>-8.3539018370624163E-3</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>0.31609548991384695</v>
+        <v>0.34631766253790586</v>
       </c>
       <c r="B24" s="1">
-        <v>10.667912115941821</v>
+        <v>10.68846691537864</v>
       </c>
       <c r="C24" s="1">
-        <v>-7.7620317288752894</v>
+        <v>-7.7281084731380254</v>
       </c>
       <c r="D24" s="1">
-        <v>5.5999999999999994E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="E24" s="1">
-        <v>3.1599513754660913E-2</v>
+        <v>6.0338543206439742E-2</v>
       </c>
       <c r="F24" s="1">
-        <v>4.3338554257067265E-2</v>
+        <v>8.3562286509440101E-2</v>
       </c>
       <c r="G24" s="1">
-        <v>-11.098364010275084</v>
+        <v>-11.113167173022466</v>
       </c>
       <c r="H24" s="1">
-        <v>6.2586816762206876</v>
+        <v>6.1818631748793136</v>
       </c>
       <c r="I24" s="1">
-        <v>-8.3539018370624163E-3</v>
+        <v>-6.1045556762068465E-2</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>0.34631766253790586</v>
+        <v>0.37119699131447775</v>
       </c>
       <c r="B25" s="1">
-        <v>10.68846691537864</v>
+        <v>10.658057446140916</v>
       </c>
       <c r="C25" s="1">
-        <v>-7.7281084731380254</v>
+        <v>-7.7539653722658368</v>
       </c>
       <c r="D25" s="1">
-        <v>4.9000000000000002E-2</v>
+        <v>5.5999999999999994E-2</v>
       </c>
       <c r="E25" s="1">
-        <v>6.0338543206439742E-2</v>
+        <v>0.10468653053384627</v>
       </c>
       <c r="F25" s="1">
-        <v>8.3562286509440101E-2</v>
+        <v>9.9808603186363989E-2</v>
       </c>
       <c r="G25" s="1">
-        <v>-11.113167173022466</v>
+        <v>-11.130109065033841</v>
       </c>
       <c r="H25" s="1">
-        <v>6.1818631748793136</v>
+        <v>5.8138336840884604</v>
       </c>
       <c r="I25" s="1">
-        <v>-6.1045556762068465E-2</v>
+        <v>-9.1620526787969947E-2</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>0.37119699131447775</v>
+        <v>0.36390847545099786</v>
       </c>
       <c r="B26" s="1">
-        <v>10.658057446140916</v>
+        <v>10.603886295039079</v>
       </c>
       <c r="C26" s="1">
-        <v>-7.7539653722658368</v>
+        <v>-7.7774899169583298</v>
       </c>
       <c r="D26" s="1">
-        <v>5.5999999999999994E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="E26" s="1">
-        <v>0.10468653053384627</v>
+        <v>8.7349152103850691E-2</v>
       </c>
       <c r="F26" s="1">
-        <v>9.9808603186363989E-2</v>
+        <v>5.6601197616907462E-2</v>
       </c>
       <c r="G26" s="1">
-        <v>-11.130109065033841</v>
+        <v>-11.056576192940479</v>
       </c>
       <c r="H26" s="1">
-        <v>5.8138336840884604</v>
+        <v>5.7692077494388805</v>
       </c>
       <c r="I26" s="1">
-        <v>-9.1620526787969947E-2</v>
+        <v>0.10548153239839531</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>0.36390847545099786</v>
+        <v>0.37344678518868013</v>
       </c>
       <c r="B27" s="1">
-        <v>10.603886295039079</v>
+        <v>10.627647470776932</v>
       </c>
       <c r="C27" s="1">
-        <v>-7.7774899169583298</v>
+        <v>-7.7463716434993026</v>
       </c>
       <c r="D27" s="1">
-        <v>8.5000000000000006E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="E27" s="1">
-        <v>8.7349152103850691E-2</v>
+        <v>5.6030392154696941E-2</v>
       </c>
       <c r="F27" s="1">
-        <v>5.6601197616907462E-2</v>
+        <v>4.9216866004878179E-2</v>
       </c>
       <c r="G27" s="1">
-        <v>-11.056576192940479</v>
+        <v>-11.067725538953699</v>
       </c>
       <c r="H27" s="1">
-        <v>5.7692077494388805</v>
+        <v>5.8822048942737455</v>
       </c>
       <c r="I27" s="1">
-        <v>0.10548153239839531</v>
+        <v>6.7507904272969821E-2</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>0.37344678518868013</v>
+        <v>0.39783500781138004</v>
       </c>
       <c r="B28" s="1">
-        <v>10.627647470776932</v>
+        <v>10.637512890038067</v>
       </c>
       <c r="C28" s="1">
-        <v>-7.7463716434993026</v>
+        <v>-7.7233384450709748</v>
       </c>
       <c r="D28" s="1">
-        <v>7.6999999999999999E-2</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="E28" s="1">
-        <v>5.6030392154696941E-2</v>
+        <v>6.3009287106290501E-2</v>
       </c>
       <c r="F28" s="1">
-        <v>4.9216866004878179E-2</v>
+        <v>5.3874317256962963E-2</v>
       </c>
       <c r="G28" s="1">
-        <v>-11.067725538953699</v>
+        <v>-11.072010994551949</v>
       </c>
       <c r="H28" s="1">
-        <v>5.8822048942737455</v>
+        <v>5.7811184413097854</v>
       </c>
       <c r="I28" s="1">
-        <v>6.7507904272969821E-2</v>
+        <v>1.9122573425090383E-2</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>0.39783500781138004</v>
+        <v>0.42067973106710416</v>
       </c>
       <c r="B29" s="1">
-        <v>10.637512890038067</v>
+        <v>10.656052753167785</v>
       </c>
       <c r="C29" s="1">
-        <v>-7.7233384450709748</v>
+        <v>-7.6918910215610712</v>
       </c>
       <c r="D29" s="1">
-        <v>7.0999999999999994E-2</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="E29" s="1">
-        <v>6.3009287106290501E-2</v>
+        <v>7.3150628393129954E-2</v>
       </c>
       <c r="F29" s="1">
-        <v>5.3874317256962963E-2</v>
+        <v>7.6271671678976111E-2</v>
       </c>
       <c r="G29" s="1">
-        <v>-11.072010994551949</v>
+        <v>-11.059426082596909</v>
       </c>
       <c r="H29" s="1">
-        <v>5.7811184413097854</v>
+        <v>5.6854162728497668</v>
       </c>
       <c r="I29" s="1">
-        <v>1.9122573425090383E-2</v>
+        <v>-7.6750848653146519E-3</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>0.42067973106710416</v>
+        <v>0.43657580355212128</v>
       </c>
       <c r="B30" s="1">
-        <v>10.656052753167785</v>
+        <v>10.655037860637208</v>
       </c>
       <c r="C30" s="1">
-        <v>-7.6918910215610712</v>
+        <v>-7.6839326033482038</v>
       </c>
       <c r="D30" s="1">
-        <v>6.0999999999999999E-2</v>
+        <v>5.9000000000000004E-2</v>
       </c>
       <c r="E30" s="1">
-        <v>7.3150628393129954E-2</v>
+        <v>9.1487772214202817E-2</v>
       </c>
       <c r="F30" s="1">
-        <v>7.6271671678976111E-2</v>
+        <v>0.10602728748016152</v>
       </c>
       <c r="G30" s="1">
-        <v>-11.059426082596909</v>
+        <v>-11.080856577160031</v>
       </c>
       <c r="H30" s="1">
-        <v>5.6854162728497668</v>
+        <v>5.664319408508363</v>
       </c>
       <c r="I30" s="1">
-        <v>-7.6750848653146519E-3</v>
+        <v>-5.882523309302945E-2</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>0.43657580355212128</v>
+        <v>0.46304478203744959</v>
       </c>
       <c r="B31" s="1">
-        <v>10.655037860637208</v>
+        <v>10.627896997245045</v>
       </c>
       <c r="C31" s="1">
-        <v>-7.6839326033482038</v>
+        <v>-7.708389869481171</v>
       </c>
       <c r="D31" s="1">
-        <v>5.9000000000000004E-2</v>
+        <v>7.2000000000000008E-2</v>
       </c>
       <c r="E31" s="1">
-        <v>9.1487772214202817E-2</v>
+        <v>0.1052676332376152</v>
       </c>
       <c r="F31" s="1">
-        <v>0.10602728748016152</v>
+        <v>0.12514691054584209</v>
       </c>
       <c r="G31" s="1">
-        <v>-11.080856577160031</v>
+        <v>-11.05666896241007</v>
       </c>
       <c r="H31" s="1">
-        <v>5.664319408508363</v>
+        <v>5.701405469574925</v>
       </c>
       <c r="I31" s="1">
-        <v>-5.882523309302945E-2</v>
+        <v>-1.6070062789247608E-2</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>0.46304478203744959</v>
+        <v>0.48992246294245312</v>
       </c>
       <c r="B32" s="1">
-        <v>10.627896997245045</v>
+        <v>10.619217830720931</v>
       </c>
       <c r="C32" s="1">
-        <v>-7.708389869481171</v>
+        <v>-7.7007461911014561</v>
       </c>
       <c r="D32" s="1">
-        <v>7.2000000000000008E-2</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="E32" s="1">
-        <v>0.1052676332376152</v>
+        <v>9.0947011017296575E-2</v>
       </c>
       <c r="F32" s="1">
-        <v>0.12514691054584209</v>
+        <v>0.15157160402051148</v>
       </c>
       <c r="G32" s="1">
-        <v>-11.05666896241007</v>
+        <v>-11.043546069446817</v>
       </c>
       <c r="H32" s="1">
-        <v>5.701405469574925</v>
+        <v>5.6855130850603972</v>
       </c>
       <c r="I32" s="1">
-        <v>-1.6070062789247608E-2</v>
+        <v>1.0919148169845627E-3</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>0.48992246294245312</v>
+        <v>0.45246732123195671</v>
       </c>
       <c r="B33" s="1">
-        <v>10.619217830720931</v>
+        <v>10.598972165790428</v>
       </c>
       <c r="C33" s="1">
-        <v>-7.7007461911014561</v>
+        <v>-7.7378059156520482</v>
       </c>
       <c r="D33" s="1">
-        <v>7.5999999999999998E-2</v>
+        <v>9.6999999999999989E-2</v>
       </c>
       <c r="E33" s="1">
-        <v>9.0947011017296575E-2</v>
+        <v>5.8564349899068543E-2</v>
       </c>
       <c r="F33" s="1">
-        <v>0.15157160402051148</v>
+        <v>0.11543998947880132</v>
       </c>
       <c r="G33" s="1">
-        <v>-11.043546069446817</v>
+        <v>-11.021605605012335</v>
       </c>
       <c r="H33" s="1">
-        <v>5.6855130850603972</v>
+        <v>5.5597904496074628</v>
       </c>
       <c r="I33" s="1">
-        <v>1.0919148169845627E-3</v>
+        <v>0.10315185436547969</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>0.45246732123195671</v>
+        <v>0.42759881948233414</v>
       </c>
       <c r="B34" s="1">
-        <v>10.598972165790428</v>
+        <v>10.589047282876439</v>
       </c>
       <c r="C34" s="1">
-        <v>-7.7378059156520482</v>
+        <v>-7.7099740887611627</v>
       </c>
       <c r="D34" s="1">
-        <v>9.6999999999999989E-2</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="E34" s="1">
-        <v>5.8564349899068543E-2</v>
+        <v>4.1803968366434727E-2</v>
       </c>
       <c r="F34" s="1">
-        <v>0.11543998947880132</v>
+        <v>8.6966968546273768E-2</v>
       </c>
       <c r="G34" s="1">
-        <v>-11.021605605012335</v>
+        <v>-10.992789267352405</v>
       </c>
       <c r="H34" s="1">
-        <v>5.5597904496074628</v>
+        <v>5.8106155786489344</v>
       </c>
       <c r="I34" s="1">
-        <v>0.10315185436547969</v>
+        <v>0.11356985059169089</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>0.42759881948233414</v>
+        <v>0.42741416917875835</v>
       </c>
       <c r="B35" s="1">
-        <v>10.589047282876439</v>
+        <v>10.622142076613578</v>
       </c>
       <c r="C35" s="1">
-        <v>-7.7099740887611627</v>
+        <v>-7.6569109143536407</v>
       </c>
       <c r="D35" s="1">
-        <v>9.6000000000000002E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="E35" s="1">
-        <v>4.1803968366434727E-2</v>
+        <v>4.010999733816524E-2</v>
       </c>
       <c r="F35" s="1">
-        <v>8.6966968546273768E-2</v>
+        <v>9.7326054214970537E-2</v>
       </c>
       <c r="G35" s="1">
-        <v>-10.992789267352405</v>
+        <v>-10.982440412249971</v>
       </c>
       <c r="H35" s="1">
-        <v>5.8106155786489344</v>
+        <v>5.7707652743550515</v>
       </c>
       <c r="I35" s="1">
-        <v>0.11356985059169089</v>
+        <v>9.8998222360106691E-2</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>0.42741416917875835</v>
+        <v>0.43513069010355893</v>
       </c>
       <c r="B36" s="1">
-        <v>10.622142076613578</v>
+        <v>10.639689560144722</v>
       </c>
       <c r="C36" s="1">
-        <v>-7.6569109143536407</v>
+        <v>-7.6327087061959027</v>
       </c>
       <c r="D36" s="1">
-        <v>7.4999999999999997E-2</v>
+        <v>7.2000000000000008E-2</v>
       </c>
       <c r="E36" s="1">
-        <v>4.010999733816524E-2</v>
+        <v>3.3762700235197299E-2</v>
       </c>
       <c r="F36" s="1">
-        <v>9.7326054214970537E-2</v>
+        <v>7.7891970679132339E-2</v>
       </c>
       <c r="G36" s="1">
-        <v>-10.982440412249971</v>
+        <v>-10.952876092617851</v>
       </c>
       <c r="H36" s="1">
-        <v>5.7707652743550515</v>
+        <v>5.8892224933704851</v>
       </c>
       <c r="I36" s="1">
-        <v>9.8998222360106691E-2</v>
+        <v>0.10203423167718562</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>0.43513069010355893</v>
+        <v>0.44011515674939156</v>
       </c>
       <c r="B37" s="1">
-        <v>10.639689560144722</v>
+        <v>10.652982861074097</v>
       </c>
       <c r="C37" s="1">
-        <v>-7.6327087061959027</v>
+        <v>-7.6159371778921496</v>
       </c>
       <c r="D37" s="1">
-        <v>7.2000000000000008E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E37" s="1">
-        <v>3.3762700235197299E-2</v>
+        <v>1.7934851679759882E-2</v>
       </c>
       <c r="F37" s="1">
-        <v>7.7891970679132339E-2</v>
+        <v>6.5815921650615741E-2</v>
       </c>
       <c r="G37" s="1">
-        <v>-10.952876092617851</v>
+        <v>-10.931924181869686</v>
       </c>
       <c r="H37" s="1">
-        <v>5.8892224933704851</v>
+        <v>6.1063305008213105</v>
       </c>
       <c r="I37" s="1">
-        <v>0.10203423167718562</v>
+        <v>9.169116988398418E-2</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>0.44011515674939156</v>
+        <v>0.39501725155114936</v>
       </c>
       <c r="B38" s="1">
-        <v>10.652982861074097</v>
+        <v>10.680730305954601</v>
       </c>
       <c r="C38" s="1">
-        <v>-7.6159371778921496</v>
+        <v>-7.5994311319134935</v>
       </c>
       <c r="D38" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="E38" s="1">
-        <v>1.7934851679759882E-2</v>
+        <v>3.3238641475733931E-2</v>
       </c>
       <c r="F38" s="1">
-        <v>6.5815921650615741E-2</v>
+        <v>6.4449354460772726E-2</v>
       </c>
       <c r="G38" s="1">
-        <v>-10.931924181869686</v>
+        <v>-10.946786739243949</v>
       </c>
       <c r="H38" s="1">
-        <v>6.1063305008213105</v>
+        <v>6.2666732237211908</v>
       </c>
       <c r="I38" s="1">
-        <v>9.169116988398418E-2</v>
+        <v>2.5907930729621054E-2</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>0.39501725155114936</v>
+        <v>0.37168795924958847</v>
       </c>
       <c r="B39" s="1">
-        <v>10.680730305954601</v>
+        <v>10.729109567572346</v>
       </c>
       <c r="C39" s="1">
-        <v>-7.5994311319134935</v>
+        <v>-7.57599211464004</v>
       </c>
       <c r="D39" s="1">
-        <v>6.2E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="E39" s="1">
-        <v>3.3238641475733931E-2</v>
+        <v>3.6071270964996058E-2</v>
       </c>
       <c r="F39" s="1">
-        <v>6.4449354460772726E-2</v>
+        <v>7.29347955058645E-2</v>
       </c>
       <c r="G39" s="1">
-        <v>-10.946786739243949</v>
+        <v>-10.962996444997568</v>
       </c>
       <c r="H39" s="1">
-        <v>6.2666732237211908</v>
+        <v>6.1543530138443741</v>
       </c>
       <c r="I39" s="1">
-        <v>2.5907930729621054E-2</v>
+        <v>2.2743008844959611E-2</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
-        <v>0.37168795924958847</v>
+        <v>0.37612227846359936</v>
       </c>
       <c r="B40" s="1">
-        <v>10.729109567572346</v>
+        <v>10.726009553798299</v>
       </c>
       <c r="C40" s="1">
-        <v>-7.57599211464004</v>
+        <v>-7.5580297868999997</v>
       </c>
       <c r="D40" s="1">
-        <v>5.5E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="E40" s="1">
-        <v>3.6071270964996058E-2</v>
+        <v>4.2205821595261997E-2</v>
       </c>
       <c r="F40" s="1">
-        <v>7.29347955058645E-2</v>
+        <v>8.8156220822364614E-2</v>
       </c>
       <c r="G40" s="1">
-        <v>-10.962996444997568</v>
+        <v>-10.961598202667114</v>
       </c>
       <c r="H40" s="1">
-        <v>6.1543530138443741</v>
+        <v>6.3066019459021811</v>
       </c>
       <c r="I40" s="1">
-        <v>2.2743008844959611E-2</v>
+        <v>6.8336635012107294E-3</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>0.37612227846359936</v>
+        <v>0.3784371668665974</v>
       </c>
       <c r="B41" s="1">
-        <v>10.726009553798299</v>
+        <v>10.718952594482573</v>
       </c>
       <c r="C41" s="1">
-        <v>-7.5580297868999997</v>
+        <v>-7.5584821461891645</v>
       </c>
       <c r="D41" s="1">
-        <v>5.2999999999999999E-2</v>
+        <v>5.5999999999999994E-2</v>
       </c>
       <c r="E41" s="1">
-        <v>4.2205821595261997E-2</v>
+        <v>4.862755335600577E-2</v>
       </c>
       <c r="F41" s="1">
-        <v>8.8156220822364614E-2</v>
+        <v>7.7876967457267923E-2</v>
       </c>
       <c r="G41" s="1">
-        <v>-10.961598202667114</v>
+        <v>-10.953489666909364</v>
       </c>
       <c r="H41" s="1">
-        <v>6.3066019459021811</v>
+        <v>6.2937366281826792</v>
       </c>
       <c r="I41" s="1">
-        <v>6.8336635012107294E-3</v>
+        <v>3.5965024109365196E-2</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>0.3784371668665974</v>
+        <v>0.38234224654098459</v>
       </c>
       <c r="B42" s="1">
-        <v>10.718952594482573</v>
+        <v>10.689917551352799</v>
       </c>
       <c r="C42" s="1">
-        <v>-7.5584821461891645</v>
+        <v>-7.5708993140229444</v>
       </c>
       <c r="D42" s="1">
-        <v>5.5999999999999994E-2</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="E42" s="1">
-        <v>4.862755335600577E-2</v>
+        <v>3.5221544159066351E-2</v>
       </c>
       <c r="F42" s="1">
-        <v>7.7876967457267923E-2</v>
+        <v>5.5301453785002792E-2</v>
       </c>
       <c r="G42" s="1">
-        <v>-10.953489666909364</v>
+        <v>-10.962972134023993</v>
       </c>
       <c r="H42" s="1">
-        <v>6.2937366281826792</v>
+        <v>6.3756777606740513</v>
       </c>
       <c r="I42" s="1">
-        <v>3.5965024109365196E-2</v>
+        <v>5.8702325966859537E-2</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>0.38234224654098459</v>
+        <v>0.38010072482747775</v>
       </c>
       <c r="B43" s="1">
-        <v>10.689917551352799</v>
+        <v>10.698260397446189</v>
       </c>
       <c r="C43" s="1">
-        <v>-7.5708993140229444</v>
+        <v>-7.5482713438296534</v>
       </c>
       <c r="D43" s="1">
-        <v>6.9000000000000006E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="E43" s="1">
-        <v>3.5221544159066351E-2</v>
+        <v>2.5070359126940306E-2</v>
       </c>
       <c r="F43" s="1">
-        <v>5.5301453785002792E-2</v>
+        <v>3.4603527627251753E-2</v>
       </c>
       <c r="G43" s="1">
-        <v>-10.962972134023993</v>
+        <v>-10.910282206927315</v>
       </c>
       <c r="H43" s="1">
-        <v>6.3756777606740513</v>
+        <v>6.4506163821879223</v>
       </c>
       <c r="I43" s="1">
-        <v>5.8702325966859537E-2</v>
+        <v>6.6528548910129714E-2</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>0.38010072482747775</v>
+        <v>0.39674551762069454</v>
       </c>
       <c r="B44" s="1">
-        <v>10.698260397446189</v>
+        <v>10.683415967220579</v>
       </c>
       <c r="C44" s="1">
-        <v>-7.5482713438296534</v>
+        <v>-7.532872631331772</v>
       </c>
       <c r="D44" s="1">
-        <v>7.4999999999999997E-2</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="E44" s="1">
-        <v>2.5070359126940306E-2</v>
+        <v>2.4391453124159263E-2</v>
       </c>
       <c r="F44" s="1">
-        <v>3.4603527627251753E-2</v>
+        <v>2.9777186417775558E-2</v>
       </c>
       <c r="G44" s="1">
-        <v>-10.910282206927315</v>
+        <v>-10.916470949957697</v>
       </c>
       <c r="H44" s="1">
-        <v>6.4506163821879223</v>
+        <v>6.5085234750986727</v>
       </c>
       <c r="I44" s="1">
-        <v>6.6528548910129714E-2</v>
+        <v>4.3785525025838545E-2</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>0.39674551762069454</v>
+        <v>0.41084329449028284</v>
       </c>
       <c r="B45" s="1">
-        <v>10.683415967220579</v>
+        <v>10.700878365794592</v>
       </c>
       <c r="C45" s="1">
-        <v>-7.532872631331772</v>
+        <v>-7.504072784933137</v>
       </c>
       <c r="D45" s="1">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="E45" s="1">
-        <v>2.4391453124159263E-2</v>
+        <v>2.1133822845679842E-2</v>
       </c>
       <c r="F45" s="1">
-        <v>2.9777186417775558E-2</v>
+        <v>4.1134243541826841E-2</v>
       </c>
       <c r="G45" s="1">
-        <v>-10.916470949957697</v>
+        <v>-10.927509051615468</v>
       </c>
       <c r="H45" s="1">
-        <v>6.5085234750986727</v>
+        <v>6.5069628323995863</v>
       </c>
       <c r="I45" s="1">
-        <v>4.3785525025838545E-2</v>
+        <v>1.3738333161166238E-2</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>0.41084329449028284</v>
+        <v>0.41232842696799682</v>
       </c>
       <c r="B46" s="1">
-        <v>10.700878365794592</v>
+        <v>10.729171059993424</v>
       </c>
       <c r="C46" s="1">
-        <v>-7.504072784933137</v>
+        <v>-7.4876712668608594</v>
       </c>
       <c r="D46" s="1">
-        <v>6.0999999999999999E-2</v>
+        <v>5.5999999999999994E-2</v>
       </c>
       <c r="E46" s="1">
-        <v>2.1133822845679842E-2</v>
+        <v>2.3827701093417957E-2</v>
       </c>
       <c r="F46" s="1">
-        <v>4.1134243541826841E-2</v>
+        <v>5.6726286800298613E-2</v>
       </c>
       <c r="G46" s="1">
-        <v>-10.927509051615468</v>
+        <v>-10.917973033062001</v>
       </c>
       <c r="H46" s="1">
-        <v>6.5069628323995863</v>
+        <v>6.645791815053296</v>
       </c>
       <c r="I46" s="1">
-        <v>1.3738333161166238E-2</v>
+        <v>6.2690768976847444E-3</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>0.41232842696799682</v>
+        <v>0.41293666866009948</v>
       </c>
       <c r="B47" s="1">
-        <v>10.729171059993424</v>
+        <v>10.752108403073604</v>
       </c>
       <c r="C47" s="1">
-        <v>-7.4876712668608594</v>
+        <v>-7.4630435535840665</v>
       </c>
       <c r="D47" s="1">
-        <v>5.5999999999999994E-2</v>
+        <v>5.4000000000000006E-2</v>
       </c>
       <c r="E47" s="1">
-        <v>2.3827701093417957E-2</v>
+        <v>2.6233857677280609E-2</v>
       </c>
       <c r="F47" s="1">
-        <v>5.6726286800298613E-2</v>
+        <v>5.1627318933740458E-2</v>
       </c>
       <c r="G47" s="1">
-        <v>-10.917973033062001</v>
+        <v>-10.925437988177062</v>
       </c>
       <c r="H47" s="1">
-        <v>6.645791815053296</v>
+        <v>6.8334727275213734</v>
       </c>
       <c r="I47" s="1">
-        <v>6.2690768976847444E-3</v>
+        <v>2.1397485165275398E-4</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>0.41293666866009948</v>
+        <v>0.42086764883328642</v>
       </c>
       <c r="B48" s="1">
-        <v>10.752108403073604</v>
+        <v>10.790928394923187</v>
       </c>
       <c r="C48" s="1">
-        <v>-7.4630435535840665</v>
+        <v>-7.4322044000426217</v>
       </c>
       <c r="D48" s="1">
-        <v>5.4000000000000006E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="E48" s="1">
-        <v>2.6233857677280609E-2</v>
+        <v>2.1397405211446448E-2</v>
       </c>
       <c r="F48" s="1">
-        <v>5.1627318933740458E-2</v>
+        <v>5.3161039968116768E-2</v>
       </c>
       <c r="G48" s="1">
-        <v>-10.925437988177062</v>
+        <v>-10.940899896287203</v>
       </c>
       <c r="H48" s="1">
-        <v>6.8334727275213734</v>
+        <v>7.0751233523212029</v>
       </c>
       <c r="I48" s="1">
-        <v>2.1397485165275398E-4</v>
+        <v>-2.8352252403202272E-2</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>0.42086764883328642</v>
+        <v>0.4236835935998105</v>
       </c>
       <c r="B49" s="1">
-        <v>10.790928394923187</v>
+        <v>10.838418412367533</v>
       </c>
       <c r="C49" s="1">
-        <v>-7.4322044000426217</v>
+        <v>-7.4012938422616088</v>
       </c>
       <c r="D49" s="1">
-        <v>4.9000000000000002E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="E49" s="1">
-        <v>2.1397405211446448E-2</v>
+        <v>1.3846107445362448E-2</v>
       </c>
       <c r="F49" s="1">
-        <v>5.3161039968116768E-2</v>
+        <v>5.2145925824000176E-2</v>
       </c>
       <c r="G49" s="1">
-        <v>-10.940899896287203</v>
+        <v>-10.949156112151034</v>
       </c>
       <c r="H49" s="1">
-        <v>7.0751233523212029</v>
+        <v>7.2784158351969852</v>
       </c>
       <c r="I49" s="1">
-        <v>-2.8352252403202272E-2</v>
+        <v>-4.0405979430615968E-2</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
-        <v>0.4236835935998105</v>
+        <v>0.427688686177354</v>
       </c>
       <c r="B50" s="1">
-        <v>10.838418412367533</v>
+        <v>10.87698870060075</v>
       </c>
       <c r="C50" s="1">
-        <v>-7.4012938422616088</v>
+        <v>-7.3655539852782477</v>
       </c>
       <c r="D50" s="1">
-        <v>4.4999999999999998E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="E50" s="1">
-        <v>1.3846107445362448E-2</v>
+        <v>2.0670375641943985E-2</v>
       </c>
       <c r="F50" s="1">
-        <v>5.2145925824000176E-2</v>
+        <v>4.8501750556989971E-2</v>
       </c>
       <c r="G50" s="1">
-        <v>-10.949156112151034</v>
+        <v>-10.942378710241902</v>
       </c>
       <c r="H50" s="1">
-        <v>7.2784158351969852</v>
+        <v>7.4590136190607019</v>
       </c>
       <c r="I50" s="1">
-        <v>-4.0405979430615968E-2</v>
+        <v>-4.9875777276131128E-2</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
-        <v>0.427688686177354</v>
+        <v>0.43031182616898783</v>
       </c>
       <c r="B51" s="1">
-        <v>10.87698870060075</v>
+        <v>10.892845343784932</v>
       </c>
       <c r="C51" s="1">
-        <v>-7.3655539852782477</v>
+        <v>-7.3419814663549632</v>
       </c>
       <c r="D51" s="1">
-        <v>4.2000000000000003E-2</v>
+        <v>0.04</v>
       </c>
       <c r="E51" s="1">
-        <v>2.0670375641943985E-2</v>
+        <v>3.2937653409408303E-2</v>
       </c>
       <c r="F51" s="1">
-        <v>4.8501750556989971E-2</v>
+        <v>6.0486272261533344E-2</v>
       </c>
       <c r="G51" s="1">
-        <v>-10.942378710241902</v>
+        <v>-10.954641042143283</v>
       </c>
       <c r="H51" s="1">
-        <v>7.4590136190607019</v>
+        <v>7.4994427918769127</v>
       </c>
       <c r="I51" s="1">
-        <v>-4.9875777276131128E-2</v>
+        <v>-0.13327347740748019</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
-        <v>0.43031182616898783</v>
+        <v>0.42061685503950175</v>
       </c>
       <c r="B52" s="1">
-        <v>10.892845343784932</v>
+        <v>10.869089835480651</v>
       </c>
       <c r="C52" s="1">
-        <v>-7.3419814663549632</v>
+        <v>-7.3515302756744481</v>
       </c>
       <c r="D52" s="1">
-        <v>0.04</v>
+        <v>4.7E-2</v>
       </c>
       <c r="E52" s="1">
-        <v>3.2937653409408303E-2</v>
+        <v>2.7731672932473E-2</v>
       </c>
       <c r="F52" s="1">
-        <v>6.0486272261533344E-2</v>
+        <v>3.806501283666866E-2</v>
       </c>
       <c r="G52" s="1">
-        <v>-10.954641042143283</v>
+        <v>-10.940953832486866</v>
       </c>
       <c r="H52" s="1">
-        <v>7.4994427918769127</v>
+        <v>7.291829807049826</v>
       </c>
       <c r="I52" s="1">
-        <v>-0.13327347740748019</v>
+        <v>-4.8653782067934692E-2</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>0.42061685503950175</v>
+        <v>0.41016961130012869</v>
       </c>
       <c r="B53" s="1">
-        <v>10.869089835480651</v>
+        <v>10.830207655413304</v>
       </c>
       <c r="C53" s="1">
-        <v>-7.3515302756744481</v>
+        <v>-7.3527225940871554</v>
       </c>
       <c r="D53" s="1">
-        <v>4.7E-2</v>
+        <v>5.7999999999999996E-2</v>
       </c>
       <c r="E53" s="1">
-        <v>2.7731672932473E-2</v>
+        <v>1.6011373577103215E-2</v>
       </c>
       <c r="F53" s="1">
-        <v>3.806501283666866E-2</v>
+        <v>1.65284952008476E-2</v>
       </c>
       <c r="G53" s="1">
-        <v>-10.940953832486866</v>
+        <v>-10.902220284211667</v>
       </c>
       <c r="H53" s="1">
-        <v>7.291829807049826</v>
+        <v>7.0957405747457791</v>
       </c>
       <c r="I53" s="1">
-        <v>-4.8653782067934692E-2</v>
+        <v>3.8542076012567428E-2</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
-        <v>0.41016961130012869</v>
+        <v>0.38528911035291014</v>
       </c>
       <c r="B54" s="1">
-        <v>10.830207655413304</v>
+        <v>10.816402753779002</v>
       </c>
       <c r="C54" s="1">
-        <v>-7.3527225940871554</v>
+        <v>-7.340241961167119</v>
       </c>
       <c r="D54" s="1">
-        <v>5.7999999999999996E-2</v>
+        <v>0.06</v>
       </c>
       <c r="E54" s="1">
-        <v>1.6011373577103215E-2</v>
+        <v>2.2097326992464507E-2</v>
       </c>
       <c r="F54" s="1">
-        <v>1.65284952008476E-2</v>
+        <v>1.1211194598449934E-2</v>
       </c>
       <c r="G54" s="1">
-        <v>-10.902220284211667</v>
+        <v>-10.857822253733477</v>
       </c>
       <c r="H54" s="1">
-        <v>7.0957405747457791</v>
+        <v>7.0410363465285366</v>
       </c>
       <c r="I54" s="1">
-        <v>3.8542076012567428E-2</v>
+        <v>6.6061086512946954E-2</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
-        <v>0.38528911035291014</v>
+        <v>0.38537716232632252</v>
       </c>
       <c r="B55" s="1">
-        <v>10.816402753779002</v>
+        <v>10.843129824695906</v>
       </c>
       <c r="C55" s="1">
-        <v>-7.340241961167119</v>
+        <v>-7.3180555774120233</v>
       </c>
       <c r="D55" s="1">
-        <v>0.06</v>
+        <v>5.5E-2</v>
       </c>
       <c r="E55" s="1">
-        <v>2.2097326992464507E-2</v>
+        <v>2.664264151038738E-2</v>
       </c>
       <c r="F55" s="1">
-        <v>1.1211194598449934E-2</v>
+        <v>1.3394140685248438E-2</v>
       </c>
       <c r="G55" s="1">
-        <v>-10.857822253733477</v>
+        <v>-10.844693603323501</v>
       </c>
       <c r="H55" s="1">
-        <v>7.0410363465285366</v>
+        <v>7.1740822112621672</v>
       </c>
       <c r="I55" s="1">
-        <v>6.6061086512946954E-2</v>
+        <v>4.4325917362218803E-2</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
-        <v>0.38537716232632252</v>
+        <v>0.38678184852876835</v>
       </c>
       <c r="B56" s="1">
-        <v>10.843129824695906</v>
+        <v>10.864732141016706</v>
       </c>
       <c r="C56" s="1">
-        <v>-7.3180555774120233</v>
+        <v>-7.2982589396913173</v>
       </c>
       <c r="D56" s="1">
-        <v>5.5E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="E56" s="1">
-        <v>2.664264151038738E-2</v>
+        <v>3.297092519633258E-2</v>
       </c>
       <c r="F56" s="1">
-        <v>1.3394140685248438E-2</v>
+        <v>3.1612910353248515E-2</v>
       </c>
       <c r="G56" s="1">
-        <v>-10.844693603323501</v>
+        <v>-10.811161153611037</v>
       </c>
       <c r="H56" s="1">
-        <v>7.1740822112621672</v>
+        <v>7.206597598693107</v>
       </c>
       <c r="I56" s="1">
-        <v>4.4325917362218803E-2</v>
+        <v>2.1422359165916394E-2</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
-        <v>0.38678184852876835</v>
+        <v>0.38913270497325753</v>
       </c>
       <c r="B57" s="1">
-        <v>10.864732141016706</v>
+        <v>10.883017168911879</v>
       </c>
       <c r="C57" s="1">
-        <v>-7.2982589396913173</v>
+        <v>-7.2887942990874963</v>
       </c>
       <c r="D57" s="1">
-        <v>5.0999999999999997E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="E57" s="1">
-        <v>3.297092519633258E-2</v>
+        <v>3.227597402844485E-2</v>
       </c>
       <c r="F57" s="1">
-        <v>3.1612910353248515E-2</v>
+        <v>4.8444059312299684E-2</v>
       </c>
       <c r="G57" s="1">
-        <v>-10.811161153611037</v>
+        <v>-10.814773827496735</v>
       </c>
       <c r="H57" s="1">
-        <v>7.206597598693107</v>
+        <v>7.2566717402260315</v>
       </c>
       <c r="I57" s="1">
-        <v>2.1422359165916394E-2</v>
+        <v>-1.0871433241555817E-2</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
-        <v>0.38913270497325753</v>
+        <v>0.38919519137981451</v>
       </c>
       <c r="B58" s="1">
-        <v>10.883017168911879</v>
+        <v>10.910952720857996</v>
       </c>
       <c r="C58" s="1">
-        <v>-7.2887942990874963</v>
+        <v>-7.2813144867873136</v>
       </c>
       <c r="D58" s="1">
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="E58" s="1">
-        <v>3.227597402844485E-2</v>
+        <v>2.7997791721781344E-2</v>
       </c>
       <c r="F58" s="1">
-        <v>4.8444059312299684E-2</v>
+        <v>4.8968308116600821E-2</v>
       </c>
       <c r="G58" s="1">
-        <v>-10.814773827496735</v>
+        <v>-10.789379530702083</v>
       </c>
       <c r="H58" s="1">
-        <v>7.2566717402260315</v>
+        <v>7.3479002134264002</v>
       </c>
       <c r="I58" s="1">
-        <v>-1.0871433241555817E-2</v>
+        <v>9.2383738942620752E-3</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
-        <v>0.38919519137981451</v>
+        <v>0.38793422753592965</v>
       </c>
       <c r="B59" s="1">
-        <v>10.910952720857996</v>
+        <v>10.857294624696955</v>
       </c>
       <c r="C59" s="1">
-        <v>-7.2813144867873136</v>
+        <v>-7.3013504342467206</v>
       </c>
       <c r="D59" s="1">
-        <v>4.5999999999999999E-2</v>
+        <v>5.7999999999999996E-2</v>
       </c>
       <c r="E59" s="1">
-        <v>2.7997791721781344E-2</v>
+        <v>3.7637632218956905E-2</v>
       </c>
       <c r="F59" s="1">
-        <v>4.8968308116600821E-2</v>
+        <v>1.9072674748401786E-2</v>
       </c>
       <c r="G59" s="1">
-        <v>-10.789379530702083</v>
+        <v>-10.757777773057809</v>
       </c>
       <c r="H59" s="1">
-        <v>7.3479002134264002</v>
+        <v>7.1200765952915628</v>
       </c>
       <c r="I59" s="1">
-        <v>9.2383738942620752E-3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" s="2">
-        <v>0.38793422753592965</v>
-      </c>
-      <c r="B60" s="1">
-        <v>10.857294624696955</v>
-      </c>
-      <c r="C60" s="1">
-        <v>-7.3013504342467206</v>
-      </c>
-      <c r="D60" s="1">
-        <v>5.7999999999999996E-2</v>
-      </c>
-      <c r="E60" s="1">
-        <v>3.7637632218956905E-2</v>
-      </c>
-      <c r="F60" s="1">
-        <v>1.9072674748401786E-2</v>
-      </c>
-      <c r="G60" s="1">
-        <v>-10.757777773057809</v>
-      </c>
-      <c r="H60" s="1">
-        <v>7.1200765952915628</v>
-      </c>
-      <c r="I60" s="1">
         <v>0.16190653547028244</v>
       </c>
     </row>

</xml_diff>